<commit_message>
changed name of files
</commit_message>
<xml_diff>
--- a/TestScenarios.xlsx
+++ b/TestScenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LENOVO PC\I\My Projects\eclipse Projects\com.amazon.webautomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D35855-9910-49C7-B108-C80C54888708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61ED5598-21E3-452F-965F-641788A13F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9ACD8313-8C04-425D-A04D-233DD4156FC9}"/>
+    <workbookView xWindow="8535" yWindow="3030" windowWidth="19830" windowHeight="11295" xr2:uid="{9ACD8313-8C04-425D-A04D-233DD4156FC9}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
     <t xml:space="preserve">Amazon Automation </t>
   </si>
   <si>
-    <t>Adding multiple items in cart and verifying sub total</t>
+    <t>Adding two items in cart and verifying sub total</t>
   </si>
 </sst>
 </file>
@@ -589,7 +589,7 @@
   <dimension ref="A1:IV41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1314,7 +1314,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>5</v>

</xml_diff>